<commit_message>
Implemented doMove and timing test
</commit_message>
<xml_diff>
--- a/Bitboards.xlsx
+++ b/Bitboards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frank\Dropbox\Private\Projekte\_GITHUB\FrankyCpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9AE55F-0A45-446B-889C-F04C4685F31B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB7FAFA-3064-4D84-99A7-127BD82581F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22739" yWindow="26" windowWidth="20081" windowHeight="16207" xr2:uid="{780AC709-DDFA-44D2-9976-760A93C8311A}"/>
   </bookViews>
@@ -852,8 +852,8 @@
   </sheetPr>
   <dimension ref="B1:AH52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -912,7 +912,7 @@
     <col min="66" max="16384" width="11.5546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K1" t="s">
         <v>67</v>
       </c>
@@ -924,7 +924,7 @@
       <c r="Q1"/>
       <c r="R1"/>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B2" s="22">
         <v>0</v>
       </c>
@@ -973,8 +973,32 @@
       <c r="R2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="T2" s="22">
+        <v>56</v>
+      </c>
+      <c r="U2" s="23">
+        <v>57</v>
+      </c>
+      <c r="V2" s="23">
+        <v>58</v>
+      </c>
+      <c r="W2" s="23">
+        <v>59</v>
+      </c>
+      <c r="X2" s="23">
+        <v>60</v>
+      </c>
+      <c r="Y2" s="23">
+        <v>61</v>
+      </c>
+      <c r="Z2" s="23">
+        <v>62</v>
+      </c>
+      <c r="AA2" s="24">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B3" s="25">
         <v>8</v>
       </c>
@@ -1023,8 +1047,32 @@
       <c r="R3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="T3" s="25">
+        <v>48</v>
+      </c>
+      <c r="U3" s="13">
+        <v>49</v>
+      </c>
+      <c r="V3" s="13">
+        <v>50</v>
+      </c>
+      <c r="W3" s="13">
+        <v>51</v>
+      </c>
+      <c r="X3" s="13">
+        <v>52</v>
+      </c>
+      <c r="Y3" s="13">
+        <v>53</v>
+      </c>
+      <c r="Z3" s="13">
+        <v>54</v>
+      </c>
+      <c r="AA3" s="26">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B4" s="25">
         <v>16</v>
       </c>
@@ -1073,8 +1121,32 @@
       <c r="R4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="T4" s="25">
+        <v>40</v>
+      </c>
+      <c r="U4" s="13">
+        <v>41</v>
+      </c>
+      <c r="V4" s="13">
+        <v>42</v>
+      </c>
+      <c r="W4" s="13">
+        <v>43</v>
+      </c>
+      <c r="X4" s="13">
+        <v>44</v>
+      </c>
+      <c r="Y4" s="13">
+        <v>45</v>
+      </c>
+      <c r="Z4" s="13">
+        <v>46</v>
+      </c>
+      <c r="AA4" s="26">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B5" s="25">
         <v>24</v>
       </c>
@@ -1123,8 +1195,32 @@
       <c r="R5" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="T5" s="25">
+        <v>32</v>
+      </c>
+      <c r="U5" s="13">
+        <v>33</v>
+      </c>
+      <c r="V5" s="13">
+        <v>34</v>
+      </c>
+      <c r="W5" s="13">
+        <v>35</v>
+      </c>
+      <c r="X5" s="13">
+        <v>36</v>
+      </c>
+      <c r="Y5" s="13">
+        <v>37</v>
+      </c>
+      <c r="Z5" s="13">
+        <v>38</v>
+      </c>
+      <c r="AA5" s="26">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B6" s="25">
         <v>32</v>
       </c>
@@ -1173,8 +1269,32 @@
       <c r="R6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="T6" s="25">
+        <v>24</v>
+      </c>
+      <c r="U6" s="13">
+        <v>25</v>
+      </c>
+      <c r="V6" s="13">
+        <v>26</v>
+      </c>
+      <c r="W6" s="13">
+        <v>27</v>
+      </c>
+      <c r="X6" s="13">
+        <v>28</v>
+      </c>
+      <c r="Y6" s="13">
+        <v>29</v>
+      </c>
+      <c r="Z6" s="13">
+        <v>30</v>
+      </c>
+      <c r="AA6" s="26">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B7" s="25">
         <v>40</v>
       </c>
@@ -1223,8 +1343,32 @@
       <c r="R7" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="T7" s="25">
+        <v>16</v>
+      </c>
+      <c r="U7" s="13">
+        <v>17</v>
+      </c>
+      <c r="V7" s="13">
+        <v>18</v>
+      </c>
+      <c r="W7" s="13">
+        <v>19</v>
+      </c>
+      <c r="X7" s="13">
+        <v>20</v>
+      </c>
+      <c r="Y7" s="13">
+        <v>21</v>
+      </c>
+      <c r="Z7" s="13">
+        <v>22</v>
+      </c>
+      <c r="AA7" s="26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B8" s="25">
         <v>48</v>
       </c>
@@ -1273,8 +1417,32 @@
       <c r="R8" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T8" s="25">
+        <v>8</v>
+      </c>
+      <c r="U8" s="13">
+        <v>9</v>
+      </c>
+      <c r="V8" s="13">
+        <v>10</v>
+      </c>
+      <c r="W8" s="13">
+        <v>11</v>
+      </c>
+      <c r="X8" s="13">
+        <v>12</v>
+      </c>
+      <c r="Y8" s="13">
+        <v>13</v>
+      </c>
+      <c r="Z8" s="13">
+        <v>14</v>
+      </c>
+      <c r="AA8" s="26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="27">
         <v>56</v>
       </c>
@@ -1323,13 +1491,37 @@
       <c r="R9" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T9" s="27">
+        <v>0</v>
+      </c>
+      <c r="U9" s="28">
+        <v>1</v>
+      </c>
+      <c r="V9" s="28">
+        <v>2</v>
+      </c>
+      <c r="W9" s="28">
+        <v>3</v>
+      </c>
+      <c r="X9" s="28">
+        <v>4</v>
+      </c>
+      <c r="Y9" s="28">
+        <v>5</v>
+      </c>
+      <c r="Z9" s="28">
+        <v>6</v>
+      </c>
+      <c r="AA9" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K10" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:27" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B11" s="14" t="s">
         <v>0</v>
       </c>
@@ -1379,7 +1571,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:27" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B12" s="17" t="s">
         <v>2</v>
       </c>
@@ -1429,7 +1621,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:27" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B13" s="17" t="s">
         <v>4</v>
       </c>
@@ -1479,7 +1671,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:27" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B14" s="17" t="s">
         <v>6</v>
       </c>
@@ -1529,7 +1721,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:27" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B15" s="17" t="s">
         <v>8</v>
       </c>
@@ -1579,7 +1771,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:27" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B16" s="17" t="s">
         <v>10</v>
       </c>
@@ -3585,6 +3777,9 @@
       <c r="AH52" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="T2:AA9">
+    <sortCondition descending="1" ref="T2:T9"/>
+  </sortState>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" fitToWidth="0" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>